<commit_message>
Couldn't get the scrolling to work. Made a skeleton storyboard for the game. Feeling the Zzz's weighing on me. Will work more tomorrow (with artists and sounds!).
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -49,7 +49,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -65,12 +65,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -93,14 +87,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +398,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +480,7 @@
       <c r="B6" s="1">
         <v>0.25</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -501,10 +494,10 @@
       <c r="B7" s="1">
         <v>0.29166666666666602</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -515,10 +508,10 @@
       <c r="B8" s="1">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -529,10 +522,10 @@
       <c r="B9" s="1">
         <v>0.375</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -543,10 +536,10 @@
       <c r="B10" s="1">
         <v>0.41666666666666602</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -557,10 +550,10 @@
       <c r="B11" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -571,10 +564,10 @@
       <c r="B12" s="1">
         <v>0.5</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -585,10 +578,10 @@
       <c r="B13" s="1">
         <v>0.54166666666666596</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -599,10 +592,10 @@
       <c r="B14" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -613,10 +606,10 @@
       <c r="B15" s="1">
         <v>0.625</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -627,10 +620,10 @@
       <c r="B16" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -641,10 +634,10 @@
       <c r="B17" s="1">
         <v>0.70833333333333304</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -655,10 +648,10 @@
       <c r="B18" s="1">
         <v>0.75</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -669,10 +662,10 @@
       <c r="B19" s="1">
         <v>0.79166666666666596</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -683,10 +676,10 @@
       <c r="B20" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -697,10 +690,10 @@
       <c r="B21" s="1">
         <v>0.875</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -711,10 +704,10 @@
       <c r="B22" s="1">
         <v>0.91666666666666596</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -725,10 +718,10 @@
       <c r="B23" s="1">
         <v>0.95833333333333304</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -739,10 +732,10 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -753,10 +746,10 @@
       <c r="B25" s="1">
         <v>1.0416666666666701</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Setup some sound, the map, some gfx. Let's do this!
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
   <si>
     <t>PST</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>SUBMIT!</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Level Des</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Finish</t>
   </si>
 </sst>
 </file>
@@ -64,13 +76,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,7 +410,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D21" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +439,7 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -441,7 +453,7 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -455,7 +467,7 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -469,7 +481,7 @@
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -483,7 +495,7 @@
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -624,7 +636,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,7 +650,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,7 +692,7 @@
         <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,8 +733,8 @@
       <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,8 +747,8 @@
       <c r="C24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>3</v>
+      <c r="D24" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,7 +761,7 @@
       <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>